<commit_message>
Commit maj diagramme & gant
</commit_message>
<xml_diff>
--- a/Rendu/GameDoc/Source/Prefabe.xlsx
+++ b/Rendu/GameDoc/Source/Prefabe.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="14055" windowHeight="6150"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Charactère</t>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>Item représenté dans les inventaires</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item; Bonnus; </t>
+  </si>
+  <si>
+    <t>Trader; Inventaire</t>
+  </si>
+  <si>
+    <t>Move; Team; Inventaire; IA</t>
+  </si>
+  <si>
+    <t>Move; Experience; Team; Inventaire; Spell</t>
   </si>
 </sst>
 </file>
@@ -179,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -203,32 +221,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -338,47 +330,84 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C24"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -685,220 +714,293 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" ht="19.5" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="8" t="s">
+      <c r="D1" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="3" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="3" t="s">
+      <c r="D5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="3" t="s">
+      <c r="D6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="3" t="s">
+      <c r="D7" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="3" t="s">
+      <c r="D8" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="3" t="s">
+      <c r="D9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="3" t="s">
+      <c r="D10" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="3" t="s">
+      <c r="D11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="4" t="s">
+      <c r="D12" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="8" t="s">
+      <c r="D13" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="12"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="3" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="4" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A16" s="9"/>
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="8" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="3" t="s">
+      <c r="D17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="3" t="s">
+      <c r="D18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="3" t="s">
+      <c r="D19" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="3" t="s">
+      <c r="D20" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="3" t="s">
+      <c r="D21" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="3" t="s">
+      <c r="D22" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A23" s="8"/>
+      <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A24" s="10"/>
-      <c r="B24" s="4" t="s">
+      <c r="D23" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A24" s="9"/>
+      <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="12" t="s">
         <v>33</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>